<commit_message>
updated the metadata in the excel file
</commit_message>
<xml_diff>
--- a/4.project.128/Metadata.xlsx
+++ b/4.project.128/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargas/padl/template-repo/4.project.XX/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palomacartwright/Documents/EDI/scripps_caselle_fish_data/4.project.128/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E96BF3C-ADBD-9D48-84E4-974ACDAF4074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1C2B76-F5F4-4046-84FA-DE6F4E9D0AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27620" windowHeight="17500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{3EE599B7-8C8A-034C-9627-5DB855A5679C}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{6A019FA2-6D1B-044B-960E-EC38D1485A09}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>For a new unit, define it in Unit Dictionary and fill in the unit id in this column</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{3EE599B7-8C8A-034C-9627-5DB855A5679C}">
       <text>
         <r>
           <rPr>
@@ -182,39 +215,6 @@
             <family val="2"/>
           </rPr>
           <t>aplicable for Date class</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{6A019FA2-6D1B-044B-960E-EC38D1485A09}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>LK:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>For a new unit, define it in Unit Dictionary and fill in the unit id in this column</t>
         </r>
       </text>
     </comment>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="1176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="1286">
   <si>
     <t>csv_E</t>
   </si>
@@ -4002,6 +4002,336 @@
   </si>
   <si>
     <t>University of Michigan</t>
+  </si>
+  <si>
+    <t>edi.1174.1</t>
+  </si>
+  <si>
+    <t>Scripps Institution of Oceanography and Caselle Lab Fish Survey Data from 2008 - Present</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>scripps_caselle_fish_data.csv</t>
+  </si>
+  <si>
+    <t>scripps_caselle_site_list.csv</t>
+  </si>
+  <si>
+    <t>scripps_caselle_taxonomy_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripps Caselle Fish Survey Data 2008 - Present </t>
+  </si>
+  <si>
+    <t>Data from surveys done by the Scripps Institute of Oceanography and the Caselle Lab at UCSB from 2008 to preset</t>
+  </si>
+  <si>
+    <t>Scripps Caselle Site List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of all the sites surveyed with geographical information for all of the surveys included in the dataset </t>
+  </si>
+  <si>
+    <t>Scripps Caselle Taxonomy Table</t>
+  </si>
+  <si>
+    <t>Taxonomic Information for all of the fish species surveyed by both the Caselle Lab and the Scripps Institute of Oceanography Team</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>What was going on this year. Who funded and under what project is the monitoring done</t>
+  </si>
+  <si>
+    <t>reef</t>
+  </si>
+  <si>
+    <t>This shows all data is from Palmyra </t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date of the survey</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Year of the survey</t>
+  </si>
+  <si>
+    <t>station</t>
+  </si>
+  <si>
+    <t>Original Station Entry</t>
+  </si>
+  <si>
+    <t>station_clean</t>
+  </si>
+  <si>
+    <t>Standardized station list which corresponds to the site_list csv. You can find all of the stations with their geographical coordinates there. </t>
+  </si>
+  <si>
+    <t>transect</t>
+  </si>
+  <si>
+    <t>Which transect the survey was completed in </t>
+  </si>
+  <si>
+    <t>diver</t>
+  </si>
+  <si>
+    <t>Initials of the diver completing the survey</t>
+  </si>
+  <si>
+    <t>depth_zn</t>
+  </si>
+  <si>
+    <t>What is the target depth of the diver for that survey</t>
+  </si>
+  <si>
+    <t>datatyp</t>
+  </si>
+  <si>
+    <t>all quantitative</t>
+  </si>
+  <si>
+    <t>Number of fish seen along the transect</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>Size estimate</t>
+  </si>
+  <si>
+    <t>size_tp</t>
+  </si>
+  <si>
+    <t>If they are in terminal phase, this is the size of the fish</t>
+  </si>
+  <si>
+    <t>no_tp</t>
+  </si>
+  <si>
+    <t>Number of fish seen in terminal phase</t>
+  </si>
+  <si>
+    <t>area surveyed</t>
+  </si>
+  <si>
+    <t>squareMeters</t>
+  </si>
+  <si>
+    <t>short version of the species name. First two characters are genus and last 4 characters are the species. Format: GG.SSSS. More information on each species can be found in the taxonomy table.   </t>
+  </si>
+  <si>
+    <t>Harmonized station list that links to station_clean in fish data</t>
+  </si>
+  <si>
+    <t>Reef Surveys were completed on</t>
+  </si>
+  <si>
+    <t>habitat_zone</t>
+  </si>
+  <si>
+    <t>Which section of the reef was surveyed</t>
+  </si>
+  <si>
+    <t>depth_zone_m</t>
+  </si>
+  <si>
+    <t>Target Depth Surveyed</t>
+  </si>
+  <si>
+    <t>lat_dd</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>long_dd</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>y_proj</t>
+  </si>
+  <si>
+    <t>x_proj</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>Which survey was being completed? </t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Notes </t>
+  </si>
+  <si>
+    <t>Six character genus species code that matches the fish data table</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>Family fish species belongs to</t>
+  </si>
+  <si>
+    <t>species_code</t>
+  </si>
+  <si>
+    <t>4 digit species code</t>
+  </si>
+  <si>
+    <t>taxon</t>
+  </si>
+  <si>
+    <t>scientific name of each fish surveyed</t>
+  </si>
+  <si>
+    <t>trophic_group</t>
+  </si>
+  <si>
+    <t>trophic group of each fish surveyed</t>
+  </si>
+  <si>
+    <t>length_type</t>
+  </si>
+  <si>
+    <t>lcf</t>
+  </si>
+  <si>
+    <t>lw_a</t>
+  </si>
+  <si>
+    <t>lw_b</t>
+  </si>
+  <si>
+    <t>QUAN</t>
+  </si>
+  <si>
+    <t>Quantitative Data </t>
+  </si>
+  <si>
+    <t>PALMYRA</t>
+  </si>
+  <si>
+    <t>Palmyra </t>
+  </si>
+  <si>
+    <t>PALMYRA_REEFER</t>
+  </si>
+  <si>
+    <t>Palmyra Reefer </t>
+  </si>
+  <si>
+    <t>SIO</t>
+  </si>
+  <si>
+    <t>Scripps Institution of Oceanography</t>
+  </si>
+  <si>
+    <t>TNC_PARC_Monitoring</t>
+  </si>
+  <si>
+    <t>The Nature Conservancy Palmyra Atoll Research Consortium Monitoring  </t>
+  </si>
+  <si>
+    <t>UCSB - CASELLE</t>
+  </si>
+  <si>
+    <t>Caselle Lab Surveys </t>
+  </si>
+  <si>
+    <t>Palmyra Reef Surveys </t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>BENTHIC</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Deep_reef_terrace</t>
+  </si>
+  <si>
+    <t>Forereef</t>
+  </si>
+  <si>
+    <t>Shallow_reef_terrace</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>WD</t>
+  </si>
+  <si>
+    <t>Piscivores</t>
+  </si>
+  <si>
+    <t>Planktivore</t>
+  </si>
+  <si>
+    <t>Primary Consumer</t>
+  </si>
+  <si>
+    <t>Secondary Consumer</t>
+  </si>
+  <si>
+    <t>pcarlson</t>
+  </si>
+  <si>
+    <t>pcartwright</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Carlson</t>
+  </si>
+  <si>
+    <t>peter.carlson@ucsb.edu</t>
+  </si>
+  <si>
+    <t>0000-0003-2893-2507</t>
+  </si>
+  <si>
+    <t>Paloma</t>
+  </si>
+  <si>
+    <t>Cartwright</t>
+  </si>
+  <si>
+    <t>palomacartwright@ucsb.edu</t>
   </si>
 </sst>
 </file>
@@ -4012,7 +4342,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -4090,6 +4420,30 @@
       <name val="Times"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4112,7 +4466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4132,6 +4486,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4415,8 +4775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4497,7 +4857,30 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="I3" s="1"/>
+      <c r="A3">
+        <v>128</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E3" s="22">
+        <v>2008</v>
+      </c>
+      <c r="F3" s="22">
+        <v>2021</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1178</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1000</v>
+      </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
@@ -4514,7 +4897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -12562,8 +12945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12650,14 +13033,77 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="16">
+      <c r="A4">
+        <v>128</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
       <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="20" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16">
+      <c r="A5">
+        <v>128</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
       <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1">
+      <c r="H5" s="20" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="16">
+      <c r="A6" s="1">
+        <v>128</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="G6" s="4"/>
+      <c r="H6" s="20" t="s">
+        <v>1181</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="F7" s="10"/>
@@ -12700,11 +13146,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12713,8 +13159,10 @@
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="47.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.5" style="1" customWidth="1"/>
-    <col min="7" max="9" width="15.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="15.83203125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -12735,10 +13183,10 @@
         <v>1006</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1009</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>824</v>
@@ -12826,10 +13274,10 @@
       <c r="E5" t="s">
         <v>1082</v>
       </c>
-      <c r="F5"/>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
+      <c r="G5"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
@@ -12847,10 +13295,10 @@
       <c r="E6" t="s">
         <v>1082</v>
       </c>
-      <c r="F6"/>
-      <c r="G6" t="s">
+      <c r="F6" t="s">
         <v>3</v>
       </c>
+      <c r="G6"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
@@ -12906,10 +13354,10 @@
       <c r="E9" t="s">
         <v>1082</v>
       </c>
-      <c r="F9"/>
-      <c r="G9" t="s">
+      <c r="F9" t="s">
         <v>1097</v>
       </c>
+      <c r="G9"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
@@ -12927,10 +13375,10 @@
       <c r="E10" t="s">
         <v>1082</v>
       </c>
-      <c r="F10"/>
-      <c r="G10" t="s">
+      <c r="F10" t="s">
         <v>327</v>
       </c>
+      <c r="G10"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
@@ -13005,10 +13453,10 @@
       <c r="E14" t="s">
         <v>1144</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14"/>
+      <c r="G14" t="s">
         <v>1093</v>
       </c>
-      <c r="G14"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15">
@@ -13045,12 +13493,12 @@
       <c r="E16" t="s">
         <v>1082</v>
       </c>
-      <c r="F16"/>
-      <c r="G16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>1097</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>110</v>
       </c>
@@ -13069,16 +13517,743 @@
       <c r="F17"/>
       <c r="G17"/>
     </row>
+    <row r="18" spans="1:9" ht="16">
+      <c r="A18" s="1">
+        <v>128</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="1:9" ht="16">
+      <c r="A19" s="1">
+        <v>128</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+    </row>
+    <row r="20" spans="1:9" ht="16">
+      <c r="A20" s="1">
+        <v>128</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20" s="23" t="s">
+        <v>1194</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:9" ht="16">
+      <c r="A21" s="1">
+        <v>128</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21" s="23" t="s">
+        <v>1194</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="1:9" ht="16">
+      <c r="A22" s="1">
+        <v>128</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:9" ht="16">
+      <c r="A23" s="1">
+        <v>128</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="1:9" ht="16">
+      <c r="A24" s="1">
+        <v>128</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="1:9" ht="16">
+      <c r="A25" s="1">
+        <v>128</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="1:9" ht="16">
+      <c r="A26" s="1">
+        <v>128</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+    </row>
+    <row r="27" spans="1:9" ht="16">
+      <c r="A27" s="1">
+        <v>128</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:9" ht="16">
+      <c r="A28" s="1">
+        <v>128</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+    </row>
+    <row r="29" spans="1:9" ht="16">
+      <c r="A29" s="1">
+        <v>128</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+    </row>
+    <row r="30" spans="1:9" ht="16">
+      <c r="A30" s="1">
+        <v>128</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+    </row>
+    <row r="31" spans="1:9" ht="16">
+      <c r="A31" s="1">
+        <v>128</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+    </row>
+    <row r="32" spans="1:9" ht="16">
+      <c r="A32" s="1">
+        <v>128</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="1:9" ht="16">
+      <c r="A33" s="1">
+        <v>128</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" customHeight="1">
+      <c r="A34" s="1">
+        <v>128</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" customHeight="1">
+      <c r="A35" s="1">
+        <v>128</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+    </row>
+    <row r="36" spans="1:9" ht="16">
+      <c r="A36" s="1">
+        <v>128</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F36"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:9" ht="16">
+      <c r="A37" s="1">
+        <v>128</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:9" ht="16">
+      <c r="A38" s="1">
+        <v>128</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:9" ht="16">
+      <c r="A39" s="1">
+        <v>128</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G39"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1">
+        <v>128</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D40"/>
+      <c r="E40" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1">
+        <v>128</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D41"/>
+      <c r="E41" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G41"/>
+    </row>
+    <row r="42" spans="1:9" ht="16">
+      <c r="A42" s="1">
+        <v>128</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F42"/>
+      <c r="G42"/>
+    </row>
+    <row r="43" spans="1:9" ht="16">
+      <c r="A43" s="1">
+        <v>128</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F43"/>
+      <c r="G43"/>
+    </row>
+    <row r="44" spans="1:9" ht="16">
+      <c r="A44" s="1">
+        <v>128</v>
+      </c>
+      <c r="B44" s="1">
+        <v>3</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F44"/>
+      <c r="G44"/>
+    </row>
+    <row r="45" spans="1:9" ht="16">
+      <c r="A45" s="1">
+        <v>128</v>
+      </c>
+      <c r="B45" s="1">
+        <v>3</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F45"/>
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="1:9" ht="16">
+      <c r="A46" s="1">
+        <v>128</v>
+      </c>
+      <c r="B46" s="1">
+        <v>3</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F46"/>
+      <c r="G46"/>
+    </row>
+    <row r="47" spans="1:9" ht="16">
+      <c r="A47" s="1">
+        <v>128</v>
+      </c>
+      <c r="B47" s="1">
+        <v>3</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F47"/>
+      <c r="G47"/>
+    </row>
+    <row r="48" spans="1:9" ht="16">
+      <c r="A48" s="1">
+        <v>128</v>
+      </c>
+      <c r="B48" s="1">
+        <v>3</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F48"/>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="1:7" ht="16">
+      <c r="A49" s="1">
+        <v>128</v>
+      </c>
+      <c r="B49" s="1">
+        <v>3</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D49" s="20"/>
+      <c r="E49" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F49"/>
+      <c r="G49"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1">
+        <v>128</v>
+      </c>
+      <c r="B50" s="1">
+        <v>3</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D50"/>
+      <c r="E50" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1">
+        <v>128</v>
+      </c>
+      <c r="B51" s="1">
+        <v>3</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D51"/>
+      <c r="E51" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1">
+        <v>128</v>
+      </c>
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D52"/>
+      <c r="E52" s="23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G52"/>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+  </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E18:E1048576" xr:uid="{F3F90F79-D594-1941-9A3A-EF9F1861D001}">
-      <formula1>"character,numeric,categorical,Date"</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from values" sqref="I2:I1048576" xr:uid="{EF3D2B7E-F801-F54D-B43E-424F59DC5B40}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from values" sqref="I2:I17 I36:I1048576" xr:uid="{EF3D2B7E-F801-F54D-B43E-424F59DC5B40}">
       <formula1>"integer,natural,real,whole"</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from values" sqref="I1" xr:uid="{81676368-8811-8245-8667-EA33212D37D5}"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from unit dictionary" sqref="G1" xr:uid="{4998F1BF-B48A-CC43-8CD0-5517B80102AD}"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from unit dictionary" sqref="F1" xr:uid="{4998F1BF-B48A-CC43-8CD0-5517B80102AD}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E53:F1048576" xr:uid="{F3F90F79-D594-1941-9A3A-EF9F1861D001}">
+      <formula1>"character,numeric,categorical,Date"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -13090,7 +14265,7 @@
           <x14:formula1>
             <xm:f>ListUnitDictionary!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>G18:G1048576</xm:sqref>
+          <xm:sqref>F53:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -13100,10 +14275,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A25" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13300,12 +14475,410 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="1">
+        <v>128</v>
+      </c>
+      <c r="B12" s="23">
+        <v>1</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>1250</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="1">
+        <v>128</v>
+      </c>
+      <c r="B13" s="23">
+        <v>1</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>128</v>
+      </c>
+      <c r="B14" s="23">
+        <v>1</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>128</v>
+      </c>
+      <c r="B15" s="23">
+        <v>1</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>1255</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>128</v>
+      </c>
+      <c r="B16" s="23">
+        <v>1</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>1257</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>128</v>
+      </c>
+      <c r="B17" s="23">
+        <v>1</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>128</v>
+      </c>
+      <c r="B18" s="23">
+        <v>1</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>128</v>
+      </c>
+      <c r="B19" s="23">
+        <v>1</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>128</v>
+      </c>
+      <c r="B20" s="23">
+        <v>1</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E20" s="23"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>128</v>
+      </c>
+      <c r="B21" s="23">
+        <v>1</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="23"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>128</v>
+      </c>
+      <c r="B22" s="23">
+        <v>1</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>1263</v>
+      </c>
+      <c r="E22" s="23"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>128</v>
+      </c>
+      <c r="B23" s="23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E23" s="23"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>128</v>
+      </c>
+      <c r="B24" s="23">
+        <v>1</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>128</v>
+      </c>
+      <c r="B25" s="23">
+        <v>2</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>128</v>
+      </c>
+      <c r="B26" s="23">
+        <v>2</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>128</v>
+      </c>
+      <c r="B27" s="23">
+        <v>2</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E27" s="23"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>128</v>
+      </c>
+      <c r="B28" s="23">
+        <v>2</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1">
+        <v>128</v>
+      </c>
+      <c r="B29" s="23">
+        <v>2</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1">
+        <v>128</v>
+      </c>
+      <c r="B30" s="23">
+        <v>2</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>128</v>
+      </c>
+      <c r="B31" s="23">
+        <v>2</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>128</v>
+      </c>
+      <c r="B32" s="23">
+        <v>3</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>128</v>
+      </c>
+      <c r="B33" s="23">
+        <v>3</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>128</v>
+      </c>
+      <c r="B34" s="23">
+        <v>3</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>128</v>
+      </c>
+      <c r="B35" s="23">
+        <v>3</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>128</v>
+      </c>
+      <c r="B36" s="23">
+        <v>3</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>128</v>
+      </c>
+      <c r="B37" s="23">
+        <v>3</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>128</v>
+      </c>
+      <c r="B38" s="23">
+        <v>3</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>1276</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13315,10 +14888,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13382,6 +14955,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>128</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -13390,10 +14974,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F013127A-4C83-524F-8DF5-99BFEE8C0FCA}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -13497,11 +15081,42 @@
       </c>
     </row>
     <row r="8" spans="1:8">
+      <c r="A8" s="1">
+        <v>128</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1277</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
+        <v>128</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <v>128</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1278</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13514,7 +15129,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13547,7 +15162,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
         <v>1134</v>
@@ -13578,10 +15193,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14061,12 +15676,51 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
+    <row r="17" spans="1:14" ht="16">
+      <c r="A17" s="10" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>1280</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>1035</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>1281</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="16">
+      <c r="A18" s="10" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>1049</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>1285</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N7" r:id="rId1" xr:uid="{94A6757E-AD30-BC4A-89EC-B34B6820E56B}"/>
+    <hyperlink ref="M17" r:id="rId2" xr:uid="{CB7629D2-C47A-4B40-8A37-036814DDA382}"/>
+    <hyperlink ref="M18" r:id="rId3" xr:uid="{D6E8B1F0-5066-964B-95CC-B925F96079A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
edits with complete dataset and updated metadata excel doc
</commit_message>
<xml_diff>
--- a/4.project.128/Metadata.xlsx
+++ b/4.project.128/Metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palomacartwright/Documents/EDI/scripps_caselle_fish_data/4.project.128/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1C2B76-F5F4-4046-84FA-DE6F4E9D0AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C48AEF-557A-5443-949A-481262BEC164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27620" windowHeight="17500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="1286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="1201">
   <si>
     <t>csv_E</t>
   </si>
@@ -3710,174 +3710,21 @@
     <t>Additional information of trees and soil samples</t>
   </si>
   <si>
-    <t>This describes the vegetation community type at the sampling location. Homo refers to homogeneous (single-species) community types, while Hetero refers to heterogeneous community types.</t>
-  </si>
-  <si>
     <t>categorical</t>
   </si>
   <si>
-    <t>This refers to whether the islet from which the sample was extracted is man-made or natural. Whether the islet is man-made or natural can affect sediment properties.</t>
-  </si>
-  <si>
-    <t>Latitudinal location of the sample</t>
-  </si>
-  <si>
     <t>numeric</t>
   </si>
   <si>
-    <t>Longitudinal location of the sample</t>
-  </si>
-  <si>
-    <t>The individual islet at Palmyra from where the sample was extracted</t>
-  </si>
-  <si>
     <t>character</t>
   </si>
   <si>
-    <t>A unique identifying code assigned to each sampling location</t>
-  </si>
-  <si>
-    <t>Dry bulk density of the soil sample, measured by dividing the dried weight of the soil sample by the volume of the soil extracted at the sampling location</t>
-  </si>
-  <si>
-    <t>The percentage of organic carbon measured or calculated from each soil sample</t>
-  </si>
-  <si>
-    <t>Observed woody vegetation species closest to soil sampling location OR wood species sampled</t>
-  </si>
-  <si>
-    <t>Type of tree at the location of the sample according to remote sensing data (Struckhoff 2019)</t>
-  </si>
-  <si>
-    <t>Woody vegetation community type at the location of the sample according to remote sensing data (Struckhoff 2019)</t>
-  </si>
-  <si>
-    <t>The year in which the sample was extracted</t>
-  </si>
-  <si>
-    <t>YYYY</t>
-  </si>
-  <si>
-    <t>Based on the soil organic carbon content, the bin that each sample was assigned to for modelling purposes. High &gt;20%; Medium 10 – 20%; Low &lt;10%</t>
-  </si>
-  <si>
-    <t>Mean dry bulk density values for each bin category</t>
-  </si>
-  <si>
-    <t>Denotes which types of samples were extracted at each location</t>
-  </si>
-  <si>
     <t>gramsPerCubicMeter</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>grain</t>
-  </si>
-  <si>
-    <t>origin</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>island</t>
-  </si>
-  <si>
-    <t>dbd</t>
-  </si>
-  <si>
-    <t>org_c_per</t>
-  </si>
-  <si>
     <t>species</t>
   </si>
   <si>
-    <t>crown_ras</t>
-  </si>
-  <si>
-    <t>com_ras</t>
-  </si>
-  <si>
-    <t>sample_yr</t>
-  </si>
-  <si>
-    <t>org_c_bin</t>
-  </si>
-  <si>
-    <t>dbd_avg</t>
-  </si>
-  <si>
-    <t>sample_type</t>
-  </si>
-  <si>
-    <t>Lagoon</t>
-  </si>
-  <si>
-    <t>Leeward</t>
-  </si>
-  <si>
-    <t>Windward</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Med</t>
-  </si>
-  <si>
-    <t>Man-made</t>
-  </si>
-  <si>
-    <t>Natural</t>
-  </si>
-  <si>
-    <t>Hetero</t>
-  </si>
-  <si>
-    <t>Homo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicates that the sample was taken on the leeward side of the island (i.e. no prevailing wind). </t>
-  </si>
-  <si>
-    <t>Indicates that the sample was taken on the windward side of the island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samples extracted closer to the interior of the atoll where the prevailing wind patterns are less likely to affect grain size. </t>
-  </si>
-  <si>
-    <t>This refers to the grain or sediment found at each sampling location, as prevailing winds can affect sediment size and other soil properties.</t>
-  </si>
-  <si>
-    <t>&gt;20% of soil organic carbon</t>
-  </si>
-  <si>
-    <t>10 – 20% of soil organic carbon</t>
-  </si>
-  <si>
-    <t>&lt; 10% of soil organic carbon</t>
-  </si>
-  <si>
-    <t>Sample extracted of a man-made islet</t>
-  </si>
-  <si>
-    <t>Sample extracted of a natural islet</t>
-  </si>
-  <si>
-    <t>homogeneous (single-species) community types</t>
-  </si>
-  <si>
-    <t>heterogeneous community types</t>
-  </si>
-  <si>
     <t>Palmyra Atoll</t>
   </si>
   <si>
@@ -4019,9 +3866,6 @@
     <t>scripps_caselle_site_list.csv</t>
   </si>
   <si>
-    <t>scripps_caselle_taxonomy_table.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scripps Caselle Fish Survey Data 2008 - Present </t>
   </si>
   <si>
@@ -4034,12 +3878,6 @@
     <t xml:space="preserve">List of all the sites surveyed with geographical information for all of the surveys included in the dataset </t>
   </si>
   <si>
-    <t>Scripps Caselle Taxonomy Table</t>
-  </si>
-  <si>
-    <t>Taxonomic Information for all of the fish species surveyed by both the Caselle Lab and the Scripps Institute of Oceanography Team</t>
-  </si>
-  <si>
     <t>project</t>
   </si>
   <si>
@@ -4070,9 +3908,6 @@
     <t>station</t>
   </si>
   <si>
-    <t>Original Station Entry</t>
-  </si>
-  <si>
     <t>station_clean</t>
   </si>
   <si>
@@ -4112,27 +3947,6 @@
     <t>Size estimate</t>
   </si>
   <si>
-    <t>size_tp</t>
-  </si>
-  <si>
-    <t>If they are in terminal phase, this is the size of the fish</t>
-  </si>
-  <si>
-    <t>no_tp</t>
-  </si>
-  <si>
-    <t>Number of fish seen in terminal phase</t>
-  </si>
-  <si>
-    <t>area surveyed</t>
-  </si>
-  <si>
-    <t>squareMeters</t>
-  </si>
-  <si>
-    <t>short version of the species name. First two characters are genus and last 4 characters are the species. Format: GG.SSSS. More information on each species can be found in the taxonomy table.   </t>
-  </si>
-  <si>
     <t>Harmonized station list that links to station_clean in fish data</t>
   </si>
   <si>
@@ -4166,12 +3980,6 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>y_proj</t>
-  </si>
-  <si>
-    <t>x_proj</t>
-  </si>
-  <si>
     <t>activity</t>
   </si>
   <si>
@@ -4184,45 +3992,6 @@
     <t>Notes </t>
   </si>
   <si>
-    <t>Six character genus species code that matches the fish data table</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t>Family fish species belongs to</t>
-  </si>
-  <si>
-    <t>species_code</t>
-  </si>
-  <si>
-    <t>4 digit species code</t>
-  </si>
-  <si>
-    <t>taxon</t>
-  </si>
-  <si>
-    <t>scientific name of each fish surveyed</t>
-  </si>
-  <si>
-    <t>trophic_group</t>
-  </si>
-  <si>
-    <t>trophic group of each fish surveyed</t>
-  </si>
-  <si>
-    <t>length_type</t>
-  </si>
-  <si>
-    <t>lcf</t>
-  </si>
-  <si>
-    <t>lw_a</t>
-  </si>
-  <si>
-    <t>lw_b</t>
-  </si>
-  <si>
     <t>QUAN</t>
   </si>
   <si>
@@ -4232,21 +4001,9 @@
     <t>PALMYRA</t>
   </si>
   <si>
-    <t>Palmyra </t>
-  </si>
-  <si>
-    <t>PALMYRA_REEFER</t>
-  </si>
-  <si>
-    <t>Palmyra Reefer </t>
-  </si>
-  <si>
     <t>SIO</t>
   </si>
   <si>
-    <t>Scripps Institution of Oceanography</t>
-  </si>
-  <si>
     <t>TNC_PARC_Monitoring</t>
   </si>
   <si>
@@ -4274,39 +4031,6 @@
     <t>FISH</t>
   </si>
   <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>Deep_reef_terrace</t>
-  </si>
-  <si>
-    <t>Forereef</t>
-  </si>
-  <si>
-    <t>Shallow_reef_terrace</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>TL</t>
-  </si>
-  <si>
-    <t>WD</t>
-  </si>
-  <si>
-    <t>Piscivores</t>
-  </si>
-  <si>
-    <t>Planktivore</t>
-  </si>
-  <si>
-    <t>Primary Consumer</t>
-  </si>
-  <si>
-    <t>Secondary Consumer</t>
-  </si>
-  <si>
     <t>pcarlson</t>
   </si>
   <si>
@@ -4332,6 +4056,27 @@
   </si>
   <si>
     <t>palomacartwright@ucsb.edu</t>
+  </si>
+  <si>
+    <t>short version of the species name. First two characters are genus and last 4 characters are the species. Format: GG.SSSS  </t>
+  </si>
+  <si>
+    <t>species_name</t>
+  </si>
+  <si>
+    <t>complete scientific name for each species </t>
+  </si>
+  <si>
+    <t>tx_area_m2</t>
+  </si>
+  <si>
+    <t>depth_actual_m</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>Scripps Institution of Oceanography Surveys</t>
   </si>
 </sst>
 </file>
@@ -4342,7 +4087,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -4383,17 +4128,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="8"/>
-      <name val="DejaVu Sans"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4466,7 +4200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4482,15 +4216,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -4860,23 +4593,23 @@
       <c r="A3">
         <v>128</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>1176</v>
+      <c r="B3" s="17" t="s">
+        <v>1125</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>1177</v>
-      </c>
-      <c r="E3" s="22">
+      <c r="D3" s="19" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E3" s="20">
         <v>2008</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="20">
         <v>2021</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>1178</v>
+        <v>1127</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>1000</v>
@@ -6221,10 +5954,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>1097</v>
+        <v>1081</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1097</v>
+        <v>1081</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>1</v>
@@ -6233,7 +5966,7 @@
         <v>438</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1141</v>
+        <v>1090</v>
       </c>
       <c r="F2" s="1">
         <v>1E-3</v>
@@ -6242,7 +5975,7 @@
         <v>368</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1097</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -12943,10 +12676,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13006,7 +12739,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
       <c r="H2" s="8" t="s">
-        <v>1143</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13030,7 +12763,7 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="8" t="s">
-        <v>1142</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16">
@@ -13044,17 +12777,17 @@
         <v>1073</v>
       </c>
       <c r="D4" t="s">
-        <v>1182</v>
+        <v>1130</v>
       </c>
       <c r="E4" t="s">
-        <v>1183</v>
+        <v>1131</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="20" t="s">
-        <v>1179</v>
+      <c r="H4" s="18" t="s">
+        <v>1128</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16">
@@ -13068,58 +12801,34 @@
         <v>1073</v>
       </c>
       <c r="D5" t="s">
-        <v>1184</v>
+        <v>1132</v>
       </c>
       <c r="E5" t="s">
-        <v>1185</v>
+        <v>1133</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="20" t="s">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="16">
-      <c r="A6" s="1">
-        <v>128</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1073</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1186</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="H5" s="18" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="F6" s="10"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="20" t="s">
-        <v>1181</v>
-      </c>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="F7" s="10"/>
       <c r="G7" s="4"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8">
-      <c r="G8" s="4"/>
-      <c r="H8" s="7"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="need a matching file type" sqref="F1" xr:uid="{4380E1FC-047D-F54D-93BE-FA4ACEBAE2DB}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="wrong input" error="wrong input" promptTitle="select value:" prompt="otherEntity (non-tabular data) or dataTable (csv or txt)" sqref="C1:C1048576" xr:uid="{20A1A553-66EC-0747-AE5C-A86CFC1D0590}">
       <formula1>"otherEntity, dataTable"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="need a matching file type" sqref="F1" xr:uid="{4380E1FC-047D-F54D-93BE-FA4ACEBAE2DB}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -13130,7 +12839,7 @@
           <x14:formula1>
             <xm:f>ListFileType!$A$2:$A$86</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F6 F8:F1048576</xm:sqref>
+          <xm:sqref>F2:F5 F7:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="datasetid doesn't match" promptTitle="Match id in DataSet Sheet" xr:uid="{B9F16F1E-E81A-2B40-AE2F-5B37AF6BEB61}">
           <x14:formula1>
@@ -13146,11 +12855,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13201,1057 +12910,600 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>110</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>1098</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="2" spans="1:11" ht="16">
+      <c r="A2" s="1">
+        <v>128</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>1078</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1079</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>110</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>1099</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1126</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1079</v>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:11" ht="16">
+      <c r="A3" s="1">
+        <v>128</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>1078</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>110</v>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:11" ht="16">
+      <c r="A4" s="1">
+        <v>128</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4" s="21" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="1:11" ht="16">
+      <c r="A5" s="1">
+        <v>128</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5" s="21" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:11" ht="16">
+      <c r="A6" s="1">
+        <v>128</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E6" s="21" t="s">
         <v>1080</v>
       </c>
-      <c r="E4" t="s">
-        <v>1079</v>
-      </c>
-      <c r="F4"/>
-      <c r="G4"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>110</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6">
-        <v>110</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>1102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
+      <c r="F6"/>
       <c r="G6"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
-        <v>110</v>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:11" ht="16">
+      <c r="A7" s="1">
+        <v>128</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1085</v>
+        <v>1</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>1080</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8">
-        <v>110</v>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="1:11" ht="16">
+      <c r="A8" s="1">
+        <v>128</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1085</v>
+        <v>1</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>1078</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9">
-        <v>110</v>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:11" ht="16">
+      <c r="A9" s="1">
+        <v>128</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>1104</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:11" ht="16">
+      <c r="A10" s="1">
+        <v>128</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>1082</v>
       </c>
-      <c r="F9" t="s">
-        <v>1097</v>
-      </c>
-      <c r="G9"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10">
-        <v>110</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>1105</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1088</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F10" t="s">
-        <v>327</v>
-      </c>
+      <c r="D10" s="18" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F10"/>
       <c r="G10"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11">
-        <v>110</v>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:11" ht="16">
+      <c r="A11" s="1">
+        <v>128</v>
       </c>
       <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>1106</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1085</v>
+        <v>1</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>1080</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12">
-        <v>110</v>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" spans="1:11" ht="16">
+      <c r="A12" s="1">
+        <v>128</v>
       </c>
       <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>1107</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F12"/>
+      <c r="D12" s="18" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>2</v>
+      </c>
       <c r="G12"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13">
-        <v>110</v>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+    </row>
+    <row r="13" spans="1:11" ht="16">
+      <c r="A13" s="1">
+        <v>128</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1091</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F13"/>
+        <v>1</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>168</v>
+      </c>
       <c r="G13"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14">
-        <v>110</v>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+    </row>
+    <row r="14" spans="1:11" ht="16">
+      <c r="A14" s="1">
+        <v>128</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>1109</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1144</v>
+        <v>1</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>1078</v>
       </c>
       <c r="F14"/>
-      <c r="G14" t="s">
-        <v>1093</v>
-      </c>
+      <c r="G14"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15">
-        <v>110</v>
+      <c r="A15" s="1">
+        <v>128</v>
       </c>
       <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15" s="21" t="s">
         <v>1079</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16">
-        <v>110</v>
+      <c r="A16" s="1">
+        <v>128</v>
       </c>
       <c r="B16" s="1">
-        <v>2</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1095</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>1097</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D16"/>
+      <c r="E16" s="21" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F16"/>
       <c r="G16"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17">
-        <v>110</v>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" s="1">
+        <v>128</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1096</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1085</v>
+      <c r="C17" s="21" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>1080</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
-    </row>
-    <row r="18" spans="1:9" ht="16">
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="1">
         <v>128</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>1189</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>1079</v>
+        <v>2</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>1078</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="1:9" ht="16">
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>128</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>1079</v>
+        <v>2</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" s="21" t="s">
+        <v>1080</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9" ht="16">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>128</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>1192</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>1193</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>1144</v>
+        <v>2</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" s="21" t="s">
+        <v>1080</v>
       </c>
       <c r="F20"/>
-      <c r="G20" s="23" t="s">
-        <v>1194</v>
-      </c>
-      <c r="H20"/>
-      <c r="I20"/>
+      <c r="G20"/>
     </row>
     <row r="21" spans="1:9" ht="16">
       <c r="A21" s="1">
         <v>128</v>
       </c>
       <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>1195</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>1196</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>1144</v>
+        <v>2</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>1078</v>
       </c>
       <c r="F21"/>
-      <c r="G21" s="23" t="s">
-        <v>1194</v>
-      </c>
-      <c r="H21"/>
-      <c r="I21"/>
+      <c r="G21"/>
     </row>
     <row r="22" spans="1:9" ht="16">
       <c r="A22" s="1">
         <v>128</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>1198</v>
-      </c>
-      <c r="E22" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>1079</v>
       </c>
-      <c r="F22"/>
+      <c r="F22" s="21" t="s">
+        <v>255</v>
+      </c>
       <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
     </row>
     <row r="23" spans="1:9" ht="16">
       <c r="A23" s="1">
         <v>128</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>1200</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F23"/>
+        <v>2</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>1165</v>
+      </c>
       <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
     </row>
     <row r="24" spans="1:9" ht="16">
       <c r="A24" s="1">
         <v>128</v>
       </c>
       <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>1202</v>
-      </c>
-      <c r="E24" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E24" s="21" t="s">
         <v>1079</v>
       </c>
-      <c r="F24"/>
+      <c r="F24" s="21" t="s">
+        <v>1165</v>
+      </c>
       <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
     </row>
     <row r="25" spans="1:9" ht="16">
       <c r="A25" s="1">
         <v>128</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>1203</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>1204</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>1085</v>
+        <v>2</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>1078</v>
       </c>
       <c r="F25"/>
       <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
     </row>
     <row r="26" spans="1:9" ht="16">
       <c r="A26" s="1">
         <v>128</v>
       </c>
       <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>1205</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>1206</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>255</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F26"/>
       <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
     </row>
     <row r="27" spans="1:9" ht="16">
-      <c r="A27" s="1">
-        <v>128</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>1207</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>1208</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>1079</v>
-      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="21"/>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
     </row>
     <row r="28" spans="1:9" ht="16">
-      <c r="A28" s="1">
-        <v>128</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>1106</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>1218</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>1085</v>
-      </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="21"/>
+      <c r="F28"/>
+      <c r="G28"/>
     </row>
     <row r="29" spans="1:9" ht="16">
-      <c r="A29" s="1">
-        <v>128</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>1209</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="21"/>
+      <c r="F29"/>
+      <c r="G29"/>
     </row>
     <row r="30" spans="1:9" ht="16">
-      <c r="A30" s="1">
-        <v>128</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>1210</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>1211</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F30" s="23" t="s">
-        <v>168</v>
-      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="21"/>
+      <c r="F30"/>
       <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
     </row>
     <row r="31" spans="1:9" ht="16">
-      <c r="A31" s="1">
-        <v>128</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>1212</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>1213</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>168</v>
-      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="21"/>
+      <c r="F31"/>
       <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
     </row>
     <row r="32" spans="1:9" ht="16">
-      <c r="A32" s="1">
-        <v>128</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>2</v>
-      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="21"/>
+      <c r="F32"/>
       <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="1:9" ht="16">
-      <c r="A33" s="1">
-        <v>128</v>
-      </c>
-      <c r="B33" s="1">
-        <v>1</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>419</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>1216</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>1217</v>
-      </c>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="21"/>
+      <c r="D33"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
       <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="1:9" ht="15" customHeight="1">
-      <c r="A34" s="1">
-        <v>128</v>
-      </c>
-      <c r="B34" s="1">
-        <v>2</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>1219</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F34"/>
+    </row>
+    <row r="34" spans="3:7">
+      <c r="C34" s="21"/>
+      <c r="D34"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
       <c r="G34"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-    </row>
-    <row r="35" spans="1:9" ht="15" customHeight="1">
-      <c r="A35" s="1">
-        <v>128</v>
-      </c>
-      <c r="B35" s="1">
-        <v>2</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>1220</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>1079</v>
-      </c>
-      <c r="F35"/>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="C35" s="21"/>
+      <c r="D35"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-    </row>
-    <row r="36" spans="1:9" ht="16">
-      <c r="A36" s="1">
-        <v>128</v>
-      </c>
-      <c r="B36" s="1">
-        <v>2</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>1222</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>1079</v>
-      </c>
-      <c r="F36"/>
-      <c r="G36"/>
-    </row>
-    <row r="37" spans="1:9" ht="16">
-      <c r="A37" s="1">
-        <v>128</v>
-      </c>
-      <c r="B37" s="1">
-        <v>2</v>
-      </c>
-      <c r="C37" s="23" t="s">
-        <v>1223</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>1224</v>
-      </c>
-      <c r="E37" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F37" s="23" t="s">
-        <v>255</v>
-      </c>
-      <c r="G37"/>
-    </row>
-    <row r="38" spans="1:9" ht="16">
-      <c r="A38" s="1">
-        <v>128</v>
-      </c>
-      <c r="B38" s="1">
-        <v>2</v>
-      </c>
-      <c r="C38" s="23" t="s">
-        <v>1225</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>1226</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F38" s="23" t="s">
-        <v>1227</v>
-      </c>
-      <c r="G38"/>
-    </row>
-    <row r="39" spans="1:9" ht="16">
-      <c r="A39" s="1">
-        <v>128</v>
-      </c>
-      <c r="B39" s="1">
-        <v>2</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>1228</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>1229</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F39" s="23" t="s">
-        <v>1227</v>
-      </c>
-      <c r="G39"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1">
-        <v>128</v>
-      </c>
-      <c r="B40" s="1">
-        <v>2</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>1230</v>
-      </c>
-      <c r="D40"/>
-      <c r="E40" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F40" s="23" t="s">
-        <v>1227</v>
-      </c>
-      <c r="G40"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="1">
-        <v>128</v>
-      </c>
-      <c r="B41" s="1">
-        <v>2</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D41"/>
-      <c r="E41" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F41" s="23" t="s">
-        <v>1227</v>
-      </c>
-      <c r="G41"/>
-    </row>
-    <row r="42" spans="1:9" ht="16">
-      <c r="A42" s="1">
-        <v>128</v>
-      </c>
-      <c r="B42" s="1">
-        <v>2</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>1233</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>1079</v>
-      </c>
-      <c r="F42"/>
-      <c r="G42"/>
-    </row>
-    <row r="43" spans="1:9" ht="16">
-      <c r="A43" s="1">
-        <v>128</v>
-      </c>
-      <c r="B43" s="1">
-        <v>2</v>
-      </c>
-      <c r="C43" s="23" t="s">
-        <v>1234</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>1235</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F43"/>
-      <c r="G43"/>
-    </row>
-    <row r="44" spans="1:9" ht="16">
-      <c r="A44" s="1">
-        <v>128</v>
-      </c>
-      <c r="B44" s="1">
-        <v>3</v>
-      </c>
-      <c r="C44" s="23" t="s">
-        <v>1106</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>1236</v>
-      </c>
-      <c r="E44" s="23" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F44"/>
-      <c r="G44"/>
-    </row>
-    <row r="45" spans="1:9" ht="16">
-      <c r="A45" s="1">
-        <v>128</v>
-      </c>
-      <c r="B45" s="1">
-        <v>3</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>1237</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>1238</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F45"/>
-      <c r="G45"/>
-    </row>
-    <row r="46" spans="1:9" ht="16">
-      <c r="A46" s="1">
-        <v>128</v>
-      </c>
-      <c r="B46" s="1">
-        <v>3</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>1239</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>1240</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F46"/>
-      <c r="G46"/>
-    </row>
-    <row r="47" spans="1:9" ht="16">
-      <c r="A47" s="1">
-        <v>128</v>
-      </c>
-      <c r="B47" s="1">
-        <v>3</v>
-      </c>
-      <c r="C47" s="23" t="s">
-        <v>1241</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>1242</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F47"/>
-      <c r="G47"/>
-    </row>
-    <row r="48" spans="1:9" ht="16">
-      <c r="A48" s="1">
-        <v>128</v>
-      </c>
-      <c r="B48" s="1">
-        <v>3</v>
-      </c>
-      <c r="C48" s="23" t="s">
-        <v>1243</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>1244</v>
-      </c>
-      <c r="E48" s="23" t="s">
-        <v>1079</v>
-      </c>
-      <c r="F48"/>
-      <c r="G48"/>
-    </row>
-    <row r="49" spans="1:7" ht="16">
-      <c r="A49" s="1">
-        <v>128</v>
-      </c>
-      <c r="B49" s="1">
-        <v>3</v>
-      </c>
-      <c r="C49" s="23" t="s">
-        <v>1245</v>
-      </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="23" t="s">
-        <v>1079</v>
-      </c>
-      <c r="F49"/>
-      <c r="G49"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="1">
-        <v>128</v>
-      </c>
-      <c r="B50" s="1">
-        <v>3</v>
-      </c>
-      <c r="C50" s="23" t="s">
-        <v>1246</v>
-      </c>
-      <c r="D50"/>
-      <c r="E50" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F50" s="23" t="s">
-        <v>1227</v>
-      </c>
-      <c r="G50"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="1">
-        <v>128</v>
-      </c>
-      <c r="B51" s="1">
-        <v>3</v>
-      </c>
-      <c r="C51" s="23" t="s">
-        <v>1247</v>
-      </c>
-      <c r="D51"/>
-      <c r="E51" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F51" s="23" t="s">
-        <v>1227</v>
-      </c>
-      <c r="G51"/>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="1">
-        <v>128</v>
-      </c>
-      <c r="B52" s="1">
-        <v>3</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>1248</v>
-      </c>
-      <c r="D52"/>
-      <c r="E52" s="23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F52" s="23" t="s">
-        <v>1227</v>
-      </c>
-      <c r="G52"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
+  <mergeCells count="4">
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from values" sqref="I2:I17 I36:I1048576" xr:uid="{EF3D2B7E-F801-F54D-B43E-424F59DC5B40}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from values" sqref="I19:I1048576" xr:uid="{EF3D2B7E-F801-F54D-B43E-424F59DC5B40}">
       <formula1>"integer,natural,real,whole"</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from values" sqref="I1" xr:uid="{81676368-8811-8245-8667-EA33212D37D5}"/>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from unit dictionary" sqref="F1" xr:uid="{4998F1BF-B48A-CC43-8CD0-5517B80102AD}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E53:F1048576" xr:uid="{F3F90F79-D594-1941-9A3A-EF9F1861D001}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E36:F1048576" xr:uid="{F3F90F79-D594-1941-9A3A-EF9F1861D001}">
       <formula1>"character,numeric,categorical,Date"</formula1>
     </dataValidation>
   </dataValidations>
@@ -14265,7 +13517,7 @@
           <x14:formula1>
             <xm:f>ListUnitDictionary!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>F53:F1048576</xm:sqref>
+          <xm:sqref>F36:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14275,10 +13527,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:A38"/>
+    <sheetView zoomScale="109" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14306,579 +13558,285 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>110</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1099</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1113</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1125</v>
+        <v>128</v>
+      </c>
+      <c r="B2" s="21">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>1173</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>110</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1099</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1114</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1123</v>
+        <v>128</v>
+      </c>
+      <c r="B3" s="21">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>1200</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
-        <v>110</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1099</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1115</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1124</v>
+        <v>128</v>
+      </c>
+      <c r="B4" s="21">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>1177</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1">
-        <v>110</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1116</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>1127</v>
+        <v>128</v>
+      </c>
+      <c r="B5" s="21">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>1179</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1">
-        <v>110</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1117</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1129</v>
+        <v>128</v>
+      </c>
+      <c r="B6" s="21">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>1180</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1">
-        <v>110</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1128</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B7" s="21">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
-        <v>110</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1130</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B8" s="21">
+        <v>1</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">
-        <v>110</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1131</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B9" s="21">
+        <v>1</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
-        <v>110</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1098</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1121</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1133</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B10" s="21">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
-        <v>110</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1098</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1122</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1132</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B11" s="21">
+        <v>1</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>128</v>
       </c>
-      <c r="B12" s="23">
-        <v>1</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>1207</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>1249</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>1250</v>
+      <c r="B12" s="21">
+        <v>1</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>128</v>
       </c>
-      <c r="B13" s="23">
-        <v>1</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>1251</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>1252</v>
-      </c>
+      <c r="B13" s="21">
+        <v>2</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>128</v>
       </c>
-      <c r="B14" s="23">
-        <v>1</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>1253</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>1254</v>
+      <c r="B14" s="21">
+        <v>2</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>1184</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>128</v>
       </c>
-      <c r="B15" s="23">
-        <v>1</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>1255</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>1256</v>
+      <c r="B15" s="21">
+        <v>2</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>1174</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="1">
-        <v>128</v>
-      </c>
-      <c r="B16" s="23">
-        <v>1</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>1257</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1">
-        <v>128</v>
-      </c>
-      <c r="B17" s="23">
-        <v>1</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>1259</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1">
-        <v>128</v>
-      </c>
-      <c r="B18" s="23">
-        <v>1</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>1251</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>1261</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1">
-        <v>128</v>
-      </c>
-      <c r="B19" s="23">
-        <v>1</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="23"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1">
-        <v>128</v>
-      </c>
-      <c r="B20" s="23">
-        <v>1</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>1262</v>
-      </c>
-      <c r="E20" s="23"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1">
-        <v>128</v>
-      </c>
-      <c r="B21" s="23">
-        <v>1</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="23"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1">
-        <v>128</v>
-      </c>
-      <c r="B22" s="23">
-        <v>1</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>1263</v>
-      </c>
-      <c r="E22" s="23"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1">
-        <v>128</v>
-      </c>
-      <c r="B23" s="23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>1157</v>
-      </c>
-      <c r="E23" s="23"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1">
-        <v>128</v>
-      </c>
-      <c r="B24" s="23">
-        <v>1</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
-        <v>128</v>
-      </c>
-      <c r="B25" s="23">
-        <v>2</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>1264</v>
-      </c>
-      <c r="E25" s="23"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1">
-        <v>128</v>
-      </c>
-      <c r="B26" s="23">
-        <v>2</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>1265</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1">
-        <v>128</v>
-      </c>
-      <c r="B27" s="23">
-        <v>2</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>1266</v>
-      </c>
-      <c r="E27" s="23"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1">
-        <v>128</v>
-      </c>
-      <c r="B28" s="23">
-        <v>2</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>1267</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1">
-        <v>128</v>
-      </c>
-      <c r="B29" s="23">
-        <v>2</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>1268</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1">
-        <v>128</v>
-      </c>
-      <c r="B30" s="23">
-        <v>2</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>1269</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1">
-        <v>128</v>
-      </c>
-      <c r="B31" s="23">
-        <v>2</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>1251</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32">
-        <v>128</v>
-      </c>
-      <c r="B32" s="23">
-        <v>3</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>1245</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>1270</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1">
-        <v>128</v>
-      </c>
-      <c r="B33" s="23">
-        <v>3</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>1245</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>1271</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1">
-        <v>128</v>
-      </c>
-      <c r="B34" s="23">
-        <v>3</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>1245</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>1272</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1">
-        <v>128</v>
-      </c>
-      <c r="B35" s="23">
-        <v>3</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>1243</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>1273</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1">
-        <v>128</v>
-      </c>
-      <c r="B36" s="23">
-        <v>3</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>1243</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>1274</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1">
-        <v>128</v>
-      </c>
-      <c r="B37" s="23">
-        <v>3</v>
-      </c>
-      <c r="C37" s="23" t="s">
-        <v>1243</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1">
-        <v>128</v>
-      </c>
-      <c r="B38" s="23">
-        <v>3</v>
-      </c>
-      <c r="C38" s="23" t="s">
-        <v>1243</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>1276</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14916,7 +13874,7 @@
         <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>1134</v>
+        <v>1083</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -14927,7 +13885,7 @@
         <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>1135</v>
+        <v>1084</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -14938,7 +13896,7 @@
         <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>1136</v>
+        <v>1085</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -14949,7 +13907,7 @@
         <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>1137</v>
+        <v>1086</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -14960,7 +13918,7 @@
         <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>1134</v>
+        <v>1083</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -14996,13 +13954,13 @@
         <v>1001</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1146</v>
+        <v>1095</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1147</v>
+        <v>1096</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1148</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -15010,7 +13968,7 @@
         <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1138</v>
+        <v>1087</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1060</v>
@@ -15021,7 +13979,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1138</v>
+        <v>1087</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1065</v>
@@ -15032,7 +13990,7 @@
         <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1139</v>
+        <v>1088</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1060</v>
@@ -15043,13 +14001,13 @@
         <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1145</v>
+        <v>1094</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1037</v>
       </c>
       <c r="E5" t="s">
-        <v>1149</v>
+        <v>1098</v>
       </c>
       <c r="F5" t="s">
         <v>1071</v>
@@ -15060,7 +14018,7 @@
         <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1140</v>
+        <v>1089</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1041</v>
@@ -15071,13 +14029,13 @@
         <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1145</v>
+        <v>1094</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1030</v>
       </c>
       <c r="E7" t="s">
-        <v>1150</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -15085,10 +14043,10 @@
         <v>128</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1138</v>
+        <v>1087</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1277</v>
+        <v>1185</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -15101,7 +14059,7 @@
         <v>128</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1140</v>
+        <v>1089</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1041</v>
@@ -15112,10 +14070,10 @@
         <v>128</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1140</v>
+        <v>1089</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1278</v>
+        <v>1186</v>
       </c>
     </row>
   </sheetData>
@@ -15165,7 +14123,7 @@
         <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>1134</v>
+        <v>1083</v>
       </c>
       <c r="C2" s="5">
         <v>5.8833299999999999</v>
@@ -15195,7 +14153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -15264,7 +14222,7 @@
         <v>1033</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>1034</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -15277,7 +14235,7 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="13" t="s">
         <v>1036</v>
       </c>
       <c r="N2" s="10"/>
@@ -15288,11 +14246,11 @@
       <c r="A3" s="10" t="s">
         <v>1037</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>1038</v>
       </c>
       <c r="C3" s="10"/>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>1039</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -15305,10 +14263,10 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="13" t="s">
         <v>1040</v>
       </c>
-      <c r="N3" s="15"/>
+      <c r="N3" s="13"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
@@ -15316,11 +14274,11 @@
       <c r="A4" s="10" t="s">
         <v>1041</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>1042</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="13" t="s">
         <v>1043</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -15344,11 +14302,11 @@
       <c r="A5" s="10" t="s">
         <v>1046</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>1047</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="13" t="s">
         <v>1048</v>
       </c>
       <c r="E5" s="10" t="s">
@@ -15377,17 +14335,17 @@
       <c r="D6" s="10" t="s">
         <v>1052</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="13" t="s">
         <v>1053</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="13" t="s">
         <v>1054</v>
       </c>
       <c r="N6" s="10"/>
@@ -15421,8 +14379,8 @@
       <c r="N7" s="4" t="s">
         <v>1059</v>
       </c>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="10" t="s">
@@ -15486,14 +14444,14 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="10" t="s">
-        <v>1151</v>
+        <v>1100</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>1152</v>
+        <v>1101</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>1153</v>
+        <v>1102</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>1035</v>
@@ -15503,10 +14461,10 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="17"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10" t="s">
-        <v>1154</v>
+        <v>1103</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
@@ -15514,16 +14472,16 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="10" t="s">
-        <v>1155</v>
+        <v>1104</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>1156</v>
+        <v>1105</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>1157</v>
+        <v>1106</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>1158</v>
+        <v>1107</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>1035</v>
@@ -15533,10 +14491,10 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="17"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10" t="s">
-        <v>1159</v>
+        <v>1108</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
@@ -15544,16 +14502,16 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="10" t="s">
-        <v>1160</v>
+        <v>1109</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>1161</v>
+        <v>1110</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>1162</v>
+        <v>1111</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>1035</v>
@@ -15563,10 +14521,10 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="17"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10" t="s">
-        <v>1163</v>
+        <v>1112</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -15574,24 +14532,24 @@
     </row>
     <row r="13" spans="1:16" ht="16">
       <c r="A13" s="10" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>1165</v>
+        <v>1113</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>1114</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="18" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="D13" s="16" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>1035</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="17"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
@@ -15600,24 +14558,24 @@
     </row>
     <row r="14" spans="1:16" ht="16">
       <c r="A14" s="10" t="s">
-        <v>1167</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>1168</v>
+        <v>1116</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>1117</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="18" t="s">
-        <v>1169</v>
-      </c>
-      <c r="E14" s="18" t="s">
+      <c r="D14" s="16" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>1035</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="17"/>
+      <c r="K14" s="15"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
@@ -15626,24 +14584,24 @@
     </row>
     <row r="15" spans="1:16" ht="16">
       <c r="A15" s="10" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>1171</v>
+        <v>1119</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>1120</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>1048</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="16" t="s">
         <v>1035</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="17"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
@@ -15652,24 +14610,24 @@
     </row>
     <row r="16" spans="1:16" ht="16">
       <c r="A16" s="10" t="s">
-        <v>1172</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>1173</v>
+        <v>1121</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>1122</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="18" t="s">
-        <v>1174</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>1175</v>
-      </c>
-      <c r="F16" s="18"/>
+      <c r="D16" s="16" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F16" s="16"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="17"/>
+      <c r="K16" s="15"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
@@ -15678,39 +14636,39 @@
     </row>
     <row r="17" spans="1:14" ht="16">
       <c r="A17" s="10" t="s">
-        <v>1277</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>1279</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>1280</v>
-      </c>
-      <c r="E17" s="18" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>1035</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>1281</v>
+        <v>1189</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>1282</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="16">
       <c r="A18" s="10" t="s">
-        <v>1278</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>1283</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>1284</v>
-      </c>
-      <c r="E18" s="18" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>1049</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>1285</v>
+        <v>1193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>